<commit_message>
Added 1 skills in Cyborg skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\10-Cyborg\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
     <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="31">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,42 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recharge </t>
+  </si>
+  <si>
+    <t>Effect name: ''Power Supply''.</t>
+  </si>
+  <si>
+    <t>[[AP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0-3 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: No ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 20 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]]</t>
+  </si>
+  <si>
+    <t>Self targeting: [[+1 ''Power Supply'' effect level ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Other entities: [[Damage: 5 light ]]</t>
   </si>
 </sst>
 </file>
@@ -155,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,11 +208,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -200,6 +251,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +592,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -546,69 +601,65 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -620,64 +671,56 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -686,42 +729,17 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in Cyborg skills doc 2 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="2-SupercapacitorBlow" sheetId="2" r:id="rId2"/>
+    <sheet name="3-CyberSlash" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
     <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -126,6 +126,63 @@
   </si>
   <si>
     <t>Other entities: [[Damage: 5 light ]]</t>
+  </si>
+  <si>
+    <t>Supercapacitor Blow</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 5 ]]</t>
+  </si>
+  <si>
+    <t>Enemies targeting: [[+4 ''Power Supply'' effect level ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>[[Damage:  3 light * ''Power Supply'' effect level ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  20-30 earth ]]</t>
+  </si>
+  <si>
+    <t>Cyber Slash</t>
+  </si>
+  <si>
+    <t>[[Damage:  2 light * ''Power Supply'' effect level ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  30-40 earth ]]</t>
+  </si>
+  <si>
+    <t>Per enemy targeting: [[+2 ''Power Supply'' effect level ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Hammer area + 2 cells on each side of the caster]]</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type and Light-type damage.                                                         The Light-type damage vary depending of the ''Power Supply'' effect level.                                                                                            Increase the ''Power Supply'' level effect of the caster.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage to another entity                                                               OR                                                                                                                Increase the ''Power Supply'' effect level of the caster.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type and Light-type damage.                                                         The Light-type damage vary depending of the ''Power Supply'' effect level.                                                                                                     Increase the ''Power Supply'' effect level of the caster depending of the amount of enemies hit.</t>
   </si>
 </sst>
 </file>
@@ -191,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -223,11 +280,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -255,6 +338,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -601,9 +689,11 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -966,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +1079,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -998,43 +1088,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1046,134 +1134,89 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1183,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1249,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1215,43 +1258,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1263,71 +1304,63 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1338,59 +1371,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 3 new skills in Cyborg skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
     <sheet name="2-SupercapacitorBlow" sheetId="2" r:id="rId2"/>
     <sheet name="3-CyberSlash" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="4-TaserSword" sheetId="4" r:id="rId4"/>
+    <sheet name="5-GrapnelHook" sheetId="5" r:id="rId5"/>
+    <sheet name="6-Jetpack" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -183,6 +183,111 @@
   </si>
   <si>
     <t>Inflicts Earth-type and Light-type damage.                                                         The Light-type damage vary depending of the ''Power Supply'' effect level.                                                                                                     Increase the ''Power Supply'' effect level of the caster depending of the amount of enemies hit.</t>
+  </si>
+  <si>
+    <t>Taser Sword</t>
+  </si>
+  <si>
+    <t>[[Damage:  5 * (''Power Supply'' lvl effect) light ]]</t>
+  </si>
+  <si>
+    <t>If ''Power Supply'' lvl effect = 20 (max)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage:  125 fire ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  25 earth ]]</t>
+  </si>
+  <si>
+    <t>Set ''Power Supply'' lvl effect to 0.</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type, Light-type and Fire-Type damage.                                                         The Light-type damage vary depending of the ''Power Supply'' effect level.                                                                                                       The fire-type damage only happen when the ''Power Supply'' effect level is maxed.                                                                                                Remove all the ''Power Supply'' level of the caster.</t>
+  </si>
+  <si>
+    <t>Grapnel Hook</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 2-4 ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 2 ]]</t>
+  </si>
+  <si>
+    <t>Target: Attract by 2 cells.</t>
+  </si>
+  <si>
+    <t>On enemy: [[Damage:  10-15 earth ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and attract.</t>
+  </si>
+  <si>
+    <t>Jetpack</t>
+  </si>
+  <si>
+    <t>Self: Teleport to the targeted empty cell.</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Self: [[Melee Invulnerable]] (1 turn)</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Straight line of cells + adjacent cells (next turn) ]]</t>
+  </si>
+  <si>
+    <t>Self: End turn.</t>
+  </si>
+  <si>
+    <t>[[MP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-6 ]]</t>
+  </si>
+  <si>
+    <t>Self: -2 (''Power Supply'' effect lvl) per Range unit.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Melee Invulnerable''.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entities between caster and targeted cell: [[Damage:  25-30 fire ]] </t>
+  </si>
+  <si>
+    <t>Active glyph: [[Damage:  20 fire ]]</t>
+  </si>
+  <si>
+    <t>Entities around caster: Next turn: [[Damage:  30 fire ]]</t>
+  </si>
+  <si>
+    <t>Places an aggressive glyph from caster cell to targeted cell (2 turns)               (exclude targeted cell).</t>
+  </si>
+  <si>
+    <t>Teleports the caster.                                                                         Inflicts Fire-type damage to entities on the teleportation path.                        Places aggressive glyphs that inflicts Fire-type damage on the teleportation path.                                                                               The next turn, inflicts Fire-type damage on the adjacent cells.                                                                                                                              Consume ''Power Supply'' effect level depending of the target range. Can only select range that the caster as enough ''Power Supply'' effect level to be consumed.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -306,11 +411,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -343,6 +459,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1389,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1533,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1421,43 +1542,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1469,134 +1588,94 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1606,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1708,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1638,182 +1717,140 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1825,14 +1862,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" customWidth="1"/>
     <col min="4" max="6" width="2.85546875" customWidth="1"/>
     <col min="7" max="7" width="78.5703125" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
@@ -1846,7 +1883,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1855,175 +1892,179 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="156" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+    <row r="24" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="1"/>
+      <c r="C30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added 2 new skills in Cyborg skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="4-TaserSword" sheetId="4" r:id="rId4"/>
     <sheet name="5-GrapnelHook" sheetId="5" r:id="rId5"/>
     <sheet name="6-Jetpack" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
+    <sheet name="7-ChargingPoint" sheetId="7" r:id="rId7"/>
+    <sheet name="8-Electrotherapy" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -74,12 +74,6 @@
     <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
   </si>
   <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
     <t>SKILL NAME</t>
   </si>
   <si>
@@ -288,13 +282,88 @@
   </si>
   <si>
     <t>Teleports the caster.                                                                         Inflicts Fire-type damage to entities on the teleportation path.                        Places aggressive glyphs that inflicts Fire-type damage on the teleportation path.                                                                               The next turn, inflicts Fire-type damage on the adjacent cells.                                                                                                                              Consume ''Power Supply'' effect level depending of the target range. Can only select range that the caster as enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>Charging Point</t>
+  </si>
+  <si>
+    <t>[[Range: 1-2 ]]</t>
+  </si>
+  <si>
+    <t>Summons a ''Charging Point'' [[+10% summoner HP per AP consummed for the summoning, 3 AP, 0 MP, 30% earth resistence,    -15% fire resistence, -50% water resistence, 30% air resistence, 80% light resistence, 0% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Self-Destruction Countdown''.</t>
+  </si>
+  <si>
+    <t>Self: Remove all the remaning AP.</t>
+  </si>
+  <si>
+    <t>Self: -3 (''Power Supply'' effect lvl).</t>
+  </si>
+  <si>
+    <t>Charging Point: +1 (''Self-Destruction Countdown'' lvl effect) per AP consummed for the summoning.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Binding''.</t>
+  </si>
+  <si>
+    <t>Charging Point: [[Binding]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Charging Point skill</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Charging Point''.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Square of 1 cell around the summpn ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entities: +2 AP                                              </t>
+  </si>
+  <si>
+    <t>If character entity = ''Cyborg''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    entity: +2 (''Power Supply'' effect lvl).</t>
+  </si>
+  <si>
+    <t>Boost the AP of the allies and enemies ans increase the ''Power Supply'' level effect of Cyborgs.</t>
+  </si>
+  <si>
+    <t>Electrotherapy</t>
+  </si>
+  <si>
+    <t>[[Range: 0-2 ]]</t>
+  </si>
+  <si>
+    <t>Summons an unmovable ''Charging Point'' on an empty cell. Consume all the caster AP. The summon life and number of turn on the field vary depending of the amount of AP consumed.                                       The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>Heal Light-type a target.                                                                        Heals given are proportionate to the targets' maximum health.      The healing is more effective on the caster or an adjacent target.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>On caster or adjacent target: [[Heal:  10% target max HP]]</t>
+  </si>
+  <si>
+    <t>On ranged target:                    [[Heal:  5% target max HP]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +395,16 @@
       <name val="Algerian"/>
       <family val="5"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,12 +509,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,9 +523,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -464,6 +541,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,20 +892,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>19</v>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>48</v>
+      <c r="C5" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -824,77 +916,77 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
+      <c r="C14" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>28</v>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -905,15 +997,15 @@
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="12" t="s">
-        <v>29</v>
+      <c r="C20" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="12" t="s">
-        <v>30</v>
+      <c r="C21" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -930,7 +1022,7 @@
     </row>
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="1"/>
@@ -942,15 +1034,15 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>20</v>
+      <c r="C27" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -960,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,192 +1074,185 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1199,20 +1284,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>31</v>
+      <c r="C3" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>47</v>
+      <c r="C5" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1223,58 +1308,58 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>36</v>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>35</v>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1285,22 +1370,22 @@
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="14" t="s">
-        <v>42</v>
+      <c r="C17" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="15" t="s">
-        <v>38</v>
+      <c r="C18" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>37</v>
+      <c r="C19" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1317,7 +1402,7 @@
     </row>
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="1"/>
@@ -1329,15 +1414,15 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>20</v>
+      <c r="C25" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1369,20 +1454,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>40</v>
+      <c r="C3" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>49</v>
+      <c r="C5" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1393,51 +1478,51 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>45</v>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>46</v>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1448,22 +1533,22 @@
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="14" t="s">
-        <v>39</v>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="15" t="s">
-        <v>41</v>
+      <c r="C17" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>43</v>
+      <c r="C18" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1480,7 +1565,7 @@
     </row>
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="1"/>
@@ -1492,15 +1577,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="10" t="s">
-        <v>20</v>
+      <c r="C24" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1532,20 +1617,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>50</v>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>57</v>
+      <c r="C5" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1556,51 +1641,51 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>45</v>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1611,36 +1696,36 @@
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="14" t="s">
-        <v>54</v>
+      <c r="C16" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="16" t="s">
-        <v>51</v>
+      <c r="C17" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="16" t="s">
-        <v>52</v>
+      <c r="C18" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>53</v>
+      <c r="C19" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="12" t="s">
-        <v>55</v>
+      <c r="C20" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1657,7 +1742,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="1"/>
@@ -1669,13 +1754,13 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1688,7 +1773,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,20 +1792,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
+      <c r="C3" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>67</v>
+      <c r="C5" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1731,72 +1816,72 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>60</v>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>61</v>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>62</v>
+      <c r="C12" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>63</v>
+      <c r="C14" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>64</v>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
+      <c r="C17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1807,15 +1892,15 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>66</v>
+      <c r="C19" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="12" t="s">
-        <v>65</v>
+      <c r="C20" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1832,7 +1917,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="1"/>
@@ -1844,13 +1929,13 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1862,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,20 +1967,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>68</v>
+      <c r="C3" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="156" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>84</v>
+      <c r="C5" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1906,72 +1991,72 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>75</v>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>74</v>
+      <c r="C8" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>76</v>
+      <c r="C9" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
+      <c r="C13" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>78</v>
+      <c r="C15" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>72</v>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1982,59 +2067,59 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="14" t="s">
-        <v>69</v>
+      <c r="C19" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="16" t="s">
-        <v>77</v>
+      <c r="C20" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="16" t="s">
-        <v>71</v>
+      <c r="C21" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="18" t="s">
-        <v>73</v>
+      <c r="C22" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="12" t="s">
-        <v>80</v>
+      <c r="C23" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="15" t="s">
-        <v>81</v>
+      <c r="C25" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="3" t="s">
-        <v>82</v>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2051,7 +2136,7 @@
     </row>
     <row r="30" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="1"/>
@@ -2063,15 +2148,15 @@
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>79</v>
+      <c r="C32" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2081,10 +2166,323 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+      <c r="G1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="1"/>
+      <c r="C20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" ht="78.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B28" s="1"/>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B30" s="1"/>
+      <c r="C30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,148 +2501,140 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2253,42 +2643,15 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2296,12 +2659,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,409 +2683,185 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All skills doc for every class are done! Next step is to redefine correctly every effect and simplify them to they simple expression.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="6-Jetpack" sheetId="6" r:id="rId6"/>
     <sheet name="7-ChargingPoint" sheetId="7" r:id="rId7"/>
     <sheet name="8-Electrotherapy" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="9-ForceField" sheetId="9" r:id="rId9"/>
+    <sheet name="10-Checkpoint" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,59 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
   <si>
-    <t>[[MP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
-  <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Stright line of 1 cell]]</t>
   </si>
   <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Damage:  0-0 fire ]]</t>
-  </si>
-  <si>
-    <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
-    <t>Effect name: ''X''.</t>
-  </si>
-  <si>
-    <t>Unbuff ''X'' effect.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recharge </t>
   </si>
   <si>
@@ -347,9 +305,6 @@
     <t>Summons an unmovable ''Charging Point'' on an empty cell. Consume all the caster AP. The summon life and number of turn on the field vary depending of the amount of AP consumed.                                       The caster must have enough ''Power Supply'' effect level to be consumed.</t>
   </si>
   <si>
-    <t>The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
     <t>Heal Light-type a target.                                                                        Heals given are proportionate to the targets' maximum health.      The healing is more effective on the caster or an adjacent target.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
   </si>
   <si>
@@ -357,6 +312,54 @@
   </si>
   <si>
     <t>On ranged target:                    [[Heal:  5% target max HP]]</t>
+  </si>
+  <si>
+    <t>Force Field</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Circle whit 2 cells radius ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Force Field''.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Heavy''.</t>
+  </si>
+  <si>
+    <t>Entities can't enter or exit the ''Force Field'' area by themself.                                 The ''Force Field'' area move whit the entity having the effect.                           The entities on the ''Force Field'' area can't use self moving abilities except for the entity having the ''Force Field'' effect.                                                                                                     The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>Target: [[Force Field]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Entities on the area: [[Heavy]] (While in the area)</t>
+  </si>
+  <si>
+    <t>Self: -6 (''Power Supply'' effect lvl).</t>
+  </si>
+  <si>
+    <t>Checkpoint</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 3 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Checkpoint''.</t>
+  </si>
+  <si>
+    <t>Target: [[Checkpoint]] (1 turn)</t>
+  </si>
+  <si>
+    <t>If the target can't be teleported on his checkpoint (ex: entity there):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 100 light]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Save the position of the target and teleport it at that position at the end of his turn.                                                                    Inflicts Light-type damage to the target at the end of his turn if he didn't successfully teleport at his checkpoint position.                                                                                The caster must have enough ''Power Supply'' effect level to be consumed.</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -905,7 +908,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -917,14 +920,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -936,21 +939,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -962,7 +965,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -974,7 +977,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -986,7 +989,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -998,14 +1001,14 @@
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1023,7 +1026,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1035,7 +1038,7 @@
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1052,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1078,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1084,10 +1087,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1099,97 +1102,97 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
+      <c r="C18" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
+      <c r="C19" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
+      <c r="C21" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1198,61 +1201,35 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B30" s="1"/>
-      <c r="C30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1285,7 +1262,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1297,7 +1274,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1309,14 +1286,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1328,7 +1305,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1340,14 +1317,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1359,7 +1336,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1371,21 +1348,21 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="12" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1403,7 +1380,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1415,7 +1392,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1455,7 +1432,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1467,7 +1444,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1479,14 +1456,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1498,7 +1475,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1510,7 +1487,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1522,7 +1499,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1534,21 +1511,21 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="12" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1566,7 +1543,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1578,7 +1555,7 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1618,7 +1595,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1630,7 +1607,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1642,14 +1619,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1661,7 +1638,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1673,7 +1650,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1685,7 +1662,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1697,35 +1674,35 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="13" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1743,7 +1720,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1793,7 +1770,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1805,7 +1782,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1817,14 +1794,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1836,21 +1813,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1862,14 +1839,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1881,7 +1858,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1893,14 +1870,14 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1918,7 +1895,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1948,7 +1925,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1945,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1980,7 +1957,7 @@
     <row r="5" spans="2:4" ht="156" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1992,21 +1969,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2018,21 +1995,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2044,7 +2021,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2056,7 +2033,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2068,58 +2045,58 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="14" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="16" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="13" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2137,7 +2114,7 @@
     <row r="30" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -2149,7 +2126,7 @@
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -2184,7 +2161,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="18" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2199,12 +2176,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2219,12 +2196,12 @@
     <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="9" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2244,19 +2221,19 @@
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2271,19 +2248,19 @@
     <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -2293,12 +2270,12 @@
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -2313,12 +2290,12 @@
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -2336,7 +2313,7 @@
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="19" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2346,19 +2323,19 @@
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="20" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="21" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2373,35 +2350,35 @@
     <row r="20" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:8" ht="78.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="17" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="17" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2422,12 +2399,12 @@
     <row r="28" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
       <c r="C28" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -2442,24 +2419,24 @@
     <row r="30" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -2481,7 +2458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2502,7 +2479,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2514,7 +2491,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2526,14 +2503,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2545,21 +2522,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2571,14 +2548,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2590,7 +2567,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2602,21 +2579,21 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="13" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2634,7 +2611,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2661,10 +2638,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,7 +2661,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2693,10 +2670,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2708,116 +2685,108 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
+      <c r="C16" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
+      <c r="C18" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
+      <c r="C19" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2826,42 +2795,24 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B30" s="1"/>
-      <c r="C30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>